<commit_message>
TC12FieldValidationsMandatoryFieldVin:updated testdata TC13VerifyVehicleAssetstWithMandatoryAutopopulatedMetadataKeys:updated testdata and xpath TC02OperatorHasNoAccessToCreateChildAssets- given sleep in details page before clicking child
</commit_message>
<xml_diff>
--- a/zf-automation/zf-web/src/main/resources/testdata/MultipleGatewaySpreadsheets/Test_Provisioning_GatewayDetails_New.xlsx
+++ b/zf-automation/zf-web/src/main/resources/testdata/MultipleGatewaySpreadsheets/Test_Provisioning_GatewayDetails_New.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7080" tabRatio="959"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15210" windowHeight="1920" tabRatio="959"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>Gateway_Name</t>
   </si>
@@ -118,12 +119,6 @@
   </si>
   <si>
     <t>key3:value3,key4:value4</t>
-  </si>
-  <si>
-    <t>Bulk Gateway Root1</t>
-  </si>
-  <si>
-    <t>Bulk Gateway Root2</t>
   </si>
   <si>
     <t>84289957950745809008</t>
@@ -146,6 +141,9 @@
   </si>
   <si>
     <t>MAC_ID/IMEI</t>
+  </si>
+  <si>
+    <t>SingleGateway1</t>
   </si>
 </sst>
 </file>
@@ -579,7 +577,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -614,7 +612,7 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I1" t="s">
         <v>7</v>
@@ -634,13 +632,13 @@
     </row>
     <row r="2" spans="1:13" ht="38.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
         <v>22</v>
@@ -655,10 +653,10 @@
         <v>23</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J2" t="s">
         <v>24</v>
@@ -675,13 +673,13 @@
     </row>
     <row r="3" spans="1:13" ht="25.5">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
         <v>28</v>
@@ -696,10 +694,10 @@
         <v>29</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J3" t="s">
         <v>24</v>
@@ -725,7 +723,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>